<commit_message>
Update AMPL data file and log file for example 38
</commit_message>
<xml_diff>
--- a/excel-input/38-solid-ubday-overflow/38-solid-ubday-overflow.xlsx
+++ b/excel-input/38-solid-ubday-overflow/38-solid-ubday-overflow.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -673,7 +673,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -910,7 +910,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -988,7 +988,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1053,7 +1053,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1134,7 +1134,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1188,7 +1188,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1241,7 +1241,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1282,7 +1282,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1335,7 +1335,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1388,7 +1388,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1461,7 +1461,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1502,7 +1502,7 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1896,8 +1896,8 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2066,7 +2066,7 @@
   </sheetPr>
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2529,8 +2529,8 @@
   </sheetPr>
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3035,7 +3035,7 @@
   </sheetPr>
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3232,7 +3232,7 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -3364,7 +3364,7 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3465,7 +3465,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>